<commit_message>
Upload Tasx xlsx by Abdo
</commit_message>
<xml_diff>
--- a/Team_Tasks.xlsx
+++ b/Team_Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ELE_4\Prototype\Robotic_Car_TeamC1-HSHL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041949A7-E782-493D-9A63-81E84D3212D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAD47AB-960E-4950-817A-EC650C0BC495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="0" windowWidth="15090" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="100" windowWidth="22000" windowHeight="14550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Milestone</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dev Rahman </t>
+  </si>
+  <si>
+    <t>IR HOLDER</t>
   </si>
 </sst>
 </file>
@@ -439,13 +442,13 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.08984375" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -508,7 +511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -546,6 +549,17 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>